<commit_message>
modified:   02.xlsx 	modified:   src/AAS.jl 	modified:   src/ForestInventory.jl 	modified:   src/qml/aas.qml
</commit_message>
<xml_diff>
--- a/02.xlsx
+++ b/02.xlsx
@@ -1122,7 +1122,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="19" spans="1:2">

</xml_diff>